<commit_message>
feat(CAN protocol): update CAN protocal
</commit_message>
<xml_diff>
--- a/doc/Fury-CAN-protocol/fury-CAN-protocol.v2.1.xlsx
+++ b/doc/Fury-CAN-protocol/fury-CAN-protocol.v2.1.xlsx
@@ -16,18 +16,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="226">
   <si>
     <t>ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -655,10 +649,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>CAN2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Mo 0</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -687,55 +677,258 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>R</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mo 4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x186240F3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>电机控制器</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>转角传感器</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x180</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>标准帧</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>*</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>*</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mo 6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VCU</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>发送方名称</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>接收方名称</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VCU</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据信息</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>转矩</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>电机控制器状态、转速</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>电机温度、电控温度、母线电压&amp;电流</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>树莓派、K60</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>安全回路状态、油门深度、刹车深度、控制状态标志、给定转矩</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>树莓派、K60、VCU</t>
+  </si>
+  <si>
+    <t>树莓派、K60、VCU</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>树莓派、K60、VCU</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>电压、电流、SoC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>电池最高温度</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>转角、转速、有效位</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0CFFC6EF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>相对VCU</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>相对K60</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>相对树莓派</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>转角信息</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>转角传感器</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VCU,树莓派，K60</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>暂未分配</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>BMS</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>电池单体状态</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>继电器状态、充电状态信息</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x186140F3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x186340F4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>其他信息，见科列BMS协议</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>K60</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mo 7</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VCU、树莓派</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>姿态信息</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x204</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>T</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>R</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Mo 4</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x186240F3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>电机控制器</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>转角传感器</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x180</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>标准帧</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>*</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>*</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mo 6</t>
+    <t>树莓派、K60、VCU</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x203</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>树莓派，K60</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>电控</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VCU及电控信息</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2B</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>标志编码</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>油门深度</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>刹车深度</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1B</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>给定转矩</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>预留</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>标志位</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>转速</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0-100</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -743,153 +936,62 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>发送方名称</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>接收方名称</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>VCU</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>数据信息</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>转矩</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>电机控制器状态、转速</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>电机温度、电控温度、母线电压&amp;电流</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>树莓派、K60</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>安全回路状态、油门深度、刹车深度、控制状态标志、给定转矩</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>树莓派、K60、VCU</t>
-  </si>
-  <si>
-    <t>树莓派、K60、VCU</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>树莓派、K60、VCU</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>电压、电流、SoC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>电池最高温度</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>转角、转速、有效位</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x0CFFC6EF</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>相对VCU</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>相对K60</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>相对树莓派</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>转角信息</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>转角传感器</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>VCU,树莓派，K60</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BMS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>暂未分配</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BMS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>树莓派、K61、VCU</t>
-  </si>
-  <si>
-    <t>电池单体状态</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>继电器状态、充电状态信息</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x186140F3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x186340F4</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>其他信息，见科列BMS协议</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>K60</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mo 7</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>VCU、树莓派</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>姿态信息</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x204</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>T</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R</t>
+    <t>电控报警信息1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1B</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>正常/报警,解析见电控通信协议</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>电控报警信息2</t>
+  </si>
+  <si>
+    <t>1B</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0/1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BMS信息1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BMS信息2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CAN1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> allFlag=acRealiableFlag*1+acBrReliableFlag*2
++startFlag*4+runFlag*8   +driveReadyFlag*16+SafetyFlag*32
++brFlag*64+ZFAllowFlag*128
++YCAllowFlag*256;
+油门是否可靠*1+油门刹车是否匹配*2
++是否完成点火*4+使能电控输出*8
++进入待驶状态*16+安全回路正常*32
++刹车灯*64+闭合主负*128
++闭合预充*256</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>档位</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1B</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1~3</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1152,7 +1254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1250,6 +1352,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1259,6 +1373,42 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1268,31 +1418,70 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1303,90 +1492,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1511,7 +1616,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CCE8CF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1767,19 +1872,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N47"/>
+  <dimension ref="A1:N67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="B49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L53" sqref="L53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="16" customWidth="1"/>
     <col min="3" max="3" width="11.625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.375" style="14" customWidth="1"/>
     <col min="6" max="6" width="16.125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.5" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.5" style="4" bestFit="1" customWidth="1"/>
@@ -1793,43 +1898,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="80" t="s">
+      <c r="E1" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="73" t="s">
+      <c r="F1" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="74" t="s">
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="75" t="s">
+      <c r="N1" s="71" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="76"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="80"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="65"/>
       <c r="F2" s="18" t="s">
         <v>8</v>
       </c>
@@ -1851,23 +1956,23 @@
       <c r="L2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="74"/>
-      <c r="N2" s="75"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="71"/>
     </row>
     <row r="3" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="69" t="s">
+      <c r="D3" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="70" t="s">
+      <c r="E3" s="72" t="s">
         <v>22</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -1891,19 +1996,19 @@
       <c r="L3" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="M3" s="71">
+      <c r="M3" s="66">
         <v>20</v>
       </c>
-      <c r="N3" s="72">
+      <c r="N3" s="67">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="62"/>
-      <c r="B4" s="67"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="70"/>
+      <c r="A4" s="61"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="72"/>
       <c r="F4" s="4" t="s">
         <v>25</v>
       </c>
@@ -1922,16 +2027,16 @@
       <c r="K4" s="6">
         <v>0</v>
       </c>
-      <c r="M4" s="71"/>
-      <c r="N4" s="72"/>
+      <c r="M4" s="66"/>
+      <c r="N4" s="67"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="62"/>
-      <c r="B5" s="67"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="57" t="s">
+      <c r="A5" s="61"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="68" t="s">
         <v>26</v>
       </c>
       <c r="G5" s="5">
@@ -1946,16 +2051,16 @@
       <c r="L5" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="M5" s="71"/>
-      <c r="N5" s="72"/>
+      <c r="M5" s="66"/>
+      <c r="N5" s="67"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="62"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="57"/>
+      <c r="A6" s="61"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="68"/>
       <c r="G6" s="5">
         <v>5.2</v>
       </c>
@@ -1968,16 +2073,16 @@
       <c r="L6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M6" s="71"/>
-      <c r="N6" s="72"/>
+      <c r="M6" s="66"/>
+      <c r="N6" s="67"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="62"/>
-      <c r="B7" s="67"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="70"/>
-      <c r="F7" s="57"/>
+      <c r="A7" s="61"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="68"/>
       <c r="G7" s="5">
         <v>5.3</v>
       </c>
@@ -1990,16 +2095,16 @@
       <c r="L7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="M7" s="71"/>
-      <c r="N7" s="72"/>
+      <c r="M7" s="66"/>
+      <c r="N7" s="67"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="62"/>
-      <c r="B8" s="67"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="57"/>
+      <c r="A8" s="61"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="68"/>
       <c r="G8" s="5">
         <v>5.4</v>
       </c>
@@ -2012,16 +2117,16 @@
       <c r="L8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M8" s="71"/>
-      <c r="N8" s="72"/>
+      <c r="M8" s="66"/>
+      <c r="N8" s="67"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="62"/>
-      <c r="B9" s="67"/>
-      <c r="C9" s="68"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="70"/>
-      <c r="F9" s="57"/>
+      <c r="A9" s="61"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="68"/>
       <c r="G9" s="5">
         <v>5.5</v>
       </c>
@@ -2034,16 +2139,16 @@
       <c r="L9" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="M9" s="71"/>
-      <c r="N9" s="72"/>
+      <c r="M9" s="66"/>
+      <c r="N9" s="67"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="62"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="68"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="70"/>
-      <c r="F10" s="57"/>
+      <c r="A10" s="61"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="68"/>
       <c r="G10" s="5">
         <v>5.6</v>
       </c>
@@ -2056,16 +2161,16 @@
       <c r="L10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="M10" s="71"/>
-      <c r="N10" s="72"/>
+      <c r="M10" s="66"/>
+      <c r="N10" s="67"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="62"/>
-      <c r="B11" s="67"/>
-      <c r="C11" s="68"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="70"/>
-      <c r="F11" s="57"/>
+      <c r="A11" s="61"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="68"/>
       <c r="G11" s="5">
         <v>5.7</v>
       </c>
@@ -2078,16 +2183,16 @@
       <c r="L11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="M11" s="71"/>
-      <c r="N11" s="72"/>
+      <c r="M11" s="66"/>
+      <c r="N11" s="67"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="62"/>
-      <c r="B12" s="67"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="57"/>
+      <c r="A12" s="61"/>
+      <c r="B12" s="62"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="68"/>
       <c r="G12" s="5">
         <v>5.8</v>
       </c>
@@ -2100,15 +2205,15 @@
       <c r="L12" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="M12" s="71"/>
-      <c r="N12" s="72"/>
+      <c r="M12" s="66"/>
+      <c r="N12" s="67"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="62"/>
-      <c r="B13" s="67"/>
-      <c r="C13" s="68"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="70"/>
+      <c r="A13" s="61"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="72"/>
       <c r="F13" s="4" t="s">
         <v>27</v>
       </c>
@@ -2124,27 +2229,27 @@
       <c r="L13" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="M13" s="71"/>
-      <c r="N13" s="72"/>
+      <c r="M13" s="66"/>
+      <c r="N13" s="67"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="62"/>
-      <c r="B14" s="67"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="69"/>
-      <c r="E14" s="70"/>
+      <c r="A14" s="61"/>
+      <c r="B14" s="62"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="72"/>
       <c r="F14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="M14" s="71"/>
-      <c r="N14" s="72"/>
+      <c r="M14" s="66"/>
+      <c r="N14" s="67"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="62"/>
-      <c r="B15" s="67"/>
-      <c r="C15" s="68"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="70"/>
+      <c r="A15" s="61"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="72"/>
       <c r="F15" s="5" t="s">
         <v>48</v>
       </c>
@@ -2160,15 +2265,15 @@
       <c r="L15" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="M15" s="71"/>
-      <c r="N15" s="72"/>
+      <c r="M15" s="66"/>
+      <c r="N15" s="67"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="62"/>
-      <c r="B16" s="67"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="70"/>
+      <c r="A16" s="61"/>
+      <c r="B16" s="62"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="72"/>
       <c r="F16" s="5" t="s">
         <v>49</v>
       </c>
@@ -2187,23 +2292,23 @@
       <c r="K16" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="M16" s="71"/>
-      <c r="N16" s="72"/>
+      <c r="M16" s="66"/>
+      <c r="N16" s="67"/>
     </row>
     <row r="17" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="62" t="s">
+      <c r="A17" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="63" t="s">
+      <c r="B17" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="64" t="s">
+      <c r="C17" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="65" t="s">
+      <c r="D17" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="66" t="s">
+      <c r="E17" s="78" t="s">
         <v>23</v>
       </c>
       <c r="F17" s="4" t="s">
@@ -2227,19 +2332,19 @@
       <c r="L17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="M17" s="61">
+      <c r="M17" s="74">
         <v>20</v>
       </c>
-      <c r="N17" s="56">
+      <c r="N17" s="73">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="62"/>
-      <c r="B18" s="63"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="65"/>
-      <c r="E18" s="66"/>
+      <c r="A18" s="61"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="76"/>
+      <c r="D18" s="77"/>
+      <c r="E18" s="78"/>
       <c r="F18" s="4" t="s">
         <v>25</v>
       </c>
@@ -2258,16 +2363,16 @@
       <c r="K18" s="6">
         <v>0</v>
       </c>
-      <c r="M18" s="61"/>
-      <c r="N18" s="56"/>
+      <c r="M18" s="74"/>
+      <c r="N18" s="73"/>
     </row>
     <row r="19" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="62"/>
-      <c r="B19" s="63"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="57" t="s">
+      <c r="A19" s="61"/>
+      <c r="B19" s="75"/>
+      <c r="C19" s="76"/>
+      <c r="D19" s="77"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="68" t="s">
         <v>26</v>
       </c>
       <c r="G19" s="5">
@@ -2282,16 +2387,16 @@
       <c r="L19" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="M19" s="61"/>
-      <c r="N19" s="56"/>
+      <c r="M19" s="74"/>
+      <c r="N19" s="73"/>
     </row>
     <row r="20" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="62"/>
-      <c r="B20" s="63"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="66"/>
-      <c r="F20" s="57"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="75"/>
+      <c r="C20" s="76"/>
+      <c r="D20" s="77"/>
+      <c r="E20" s="78"/>
+      <c r="F20" s="68"/>
       <c r="G20" s="5">
         <v>5.2</v>
       </c>
@@ -2304,16 +2409,16 @@
       <c r="L20" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M20" s="61"/>
-      <c r="N20" s="56"/>
+      <c r="M20" s="74"/>
+      <c r="N20" s="73"/>
     </row>
     <row r="21" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="62"/>
-      <c r="B21" s="63"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="66"/>
-      <c r="F21" s="57"/>
+      <c r="A21" s="61"/>
+      <c r="B21" s="75"/>
+      <c r="C21" s="76"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="78"/>
+      <c r="F21" s="68"/>
       <c r="G21" s="5">
         <v>5.3</v>
       </c>
@@ -2326,16 +2431,16 @@
       <c r="L21" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="M21" s="61"/>
-      <c r="N21" s="56"/>
+      <c r="M21" s="74"/>
+      <c r="N21" s="73"/>
     </row>
     <row r="22" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="62"/>
-      <c r="B22" s="63"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="65"/>
-      <c r="E22" s="66"/>
-      <c r="F22" s="57"/>
+      <c r="A22" s="61"/>
+      <c r="B22" s="75"/>
+      <c r="C22" s="76"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="78"/>
+      <c r="F22" s="68"/>
       <c r="G22" s="5">
         <v>5.4</v>
       </c>
@@ -2348,16 +2453,16 @@
       <c r="L22" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M22" s="61"/>
-      <c r="N22" s="56"/>
+      <c r="M22" s="74"/>
+      <c r="N22" s="73"/>
     </row>
     <row r="23" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="62"/>
-      <c r="B23" s="63"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="57"/>
+      <c r="A23" s="61"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="77"/>
+      <c r="E23" s="78"/>
+      <c r="F23" s="68"/>
       <c r="G23" s="5">
         <v>5.5</v>
       </c>
@@ -2370,16 +2475,16 @@
       <c r="L23" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="M23" s="61"/>
-      <c r="N23" s="56"/>
+      <c r="M23" s="74"/>
+      <c r="N23" s="73"/>
     </row>
     <row r="24" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="62"/>
-      <c r="B24" s="63"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="57"/>
+      <c r="A24" s="61"/>
+      <c r="B24" s="75"/>
+      <c r="C24" s="76"/>
+      <c r="D24" s="77"/>
+      <c r="E24" s="78"/>
+      <c r="F24" s="68"/>
       <c r="G24" s="5">
         <v>5.6</v>
       </c>
@@ -2392,16 +2497,16 @@
       <c r="L24" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="M24" s="61"/>
-      <c r="N24" s="56"/>
+      <c r="M24" s="74"/>
+      <c r="N24" s="73"/>
     </row>
     <row r="25" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="62"/>
-      <c r="B25" s="63"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="65"/>
-      <c r="E25" s="66"/>
-      <c r="F25" s="57"/>
+      <c r="A25" s="61"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="76"/>
+      <c r="D25" s="77"/>
+      <c r="E25" s="78"/>
+      <c r="F25" s="68"/>
       <c r="G25" s="5">
         <v>5.7</v>
       </c>
@@ -2414,16 +2519,16 @@
       <c r="L25" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="M25" s="61"/>
-      <c r="N25" s="56"/>
+      <c r="M25" s="74"/>
+      <c r="N25" s="73"/>
     </row>
     <row r="26" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="62"/>
-      <c r="B26" s="63"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="65"/>
-      <c r="E26" s="66"/>
-      <c r="F26" s="57"/>
+      <c r="A26" s="61"/>
+      <c r="B26" s="75"/>
+      <c r="C26" s="76"/>
+      <c r="D26" s="77"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="68"/>
       <c r="G26" s="5">
         <v>5.8</v>
       </c>
@@ -2436,15 +2541,15 @@
       <c r="L26" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="M26" s="61"/>
-      <c r="N26" s="56"/>
+      <c r="M26" s="74"/>
+      <c r="N26" s="73"/>
     </row>
     <row r="27" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="62"/>
-      <c r="B27" s="63"/>
-      <c r="C27" s="64"/>
-      <c r="D27" s="65"/>
-      <c r="E27" s="66"/>
+      <c r="A27" s="61"/>
+      <c r="B27" s="75"/>
+      <c r="C27" s="76"/>
+      <c r="D27" s="77"/>
+      <c r="E27" s="78"/>
       <c r="F27" s="4" t="s">
         <v>59</v>
       </c>
@@ -2460,15 +2565,15 @@
       <c r="L27" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="M27" s="61"/>
-      <c r="N27" s="56"/>
+      <c r="M27" s="74"/>
+      <c r="N27" s="73"/>
     </row>
     <row r="28" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="62"/>
-      <c r="B28" s="63"/>
-      <c r="C28" s="64"/>
-      <c r="D28" s="65"/>
-      <c r="E28" s="66"/>
+      <c r="A28" s="61"/>
+      <c r="B28" s="75"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="77"/>
+      <c r="E28" s="78"/>
       <c r="F28" s="4" t="s">
         <v>60</v>
       </c>
@@ -2484,15 +2589,15 @@
       <c r="L28" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="M28" s="61"/>
-      <c r="N28" s="56"/>
+      <c r="M28" s="74"/>
+      <c r="N28" s="73"/>
     </row>
     <row r="29" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="62"/>
-      <c r="B29" s="63"/>
-      <c r="C29" s="64"/>
-      <c r="D29" s="65"/>
-      <c r="E29" s="66"/>
+      <c r="A29" s="61"/>
+      <c r="B29" s="75"/>
+      <c r="C29" s="76"/>
+      <c r="D29" s="77"/>
+      <c r="E29" s="78"/>
       <c r="F29" s="4" t="s">
         <v>61</v>
       </c>
@@ -2508,15 +2613,15 @@
       <c r="L29" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="M29" s="61"/>
-      <c r="N29" s="56"/>
+      <c r="M29" s="74"/>
+      <c r="N29" s="73"/>
     </row>
     <row r="30" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="62"/>
-      <c r="B30" s="63"/>
-      <c r="C30" s="64"/>
-      <c r="D30" s="65"/>
-      <c r="E30" s="66"/>
+      <c r="A30" s="61"/>
+      <c r="B30" s="75"/>
+      <c r="C30" s="76"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="78"/>
       <c r="F30" s="4" t="s">
         <v>62</v>
       </c>
@@ -2532,15 +2637,15 @@
       <c r="L30" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M30" s="61"/>
-      <c r="N30" s="56"/>
+      <c r="M30" s="74"/>
+      <c r="N30" s="73"/>
     </row>
     <row r="31" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="62"/>
-      <c r="B31" s="63"/>
-      <c r="C31" s="64"/>
-      <c r="D31" s="65"/>
-      <c r="E31" s="66"/>
+      <c r="A31" s="61"/>
+      <c r="B31" s="75"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="78"/>
       <c r="F31" s="4" t="s">
         <v>63</v>
       </c>
@@ -2556,15 +2661,15 @@
       <c r="L31" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M31" s="61"/>
-      <c r="N31" s="56"/>
+      <c r="M31" s="74"/>
+      <c r="N31" s="73"/>
     </row>
     <row r="32" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="62"/>
-      <c r="B32" s="63"/>
-      <c r="C32" s="64"/>
-      <c r="D32" s="65"/>
-      <c r="E32" s="66"/>
+      <c r="A32" s="61"/>
+      <c r="B32" s="75"/>
+      <c r="C32" s="76"/>
+      <c r="D32" s="77"/>
+      <c r="E32" s="78"/>
       <c r="F32" s="4" t="s">
         <v>64</v>
       </c>
@@ -2580,15 +2685,15 @@
       <c r="L32" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M32" s="61"/>
-      <c r="N32" s="56"/>
+      <c r="M32" s="74"/>
+      <c r="N32" s="73"/>
     </row>
     <row r="33" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="62"/>
-      <c r="B33" s="63"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="65"/>
-      <c r="E33" s="66"/>
+      <c r="A33" s="61"/>
+      <c r="B33" s="75"/>
+      <c r="C33" s="76"/>
+      <c r="D33" s="77"/>
+      <c r="E33" s="78"/>
       <c r="F33" s="4" t="s">
         <v>65</v>
       </c>
@@ -2604,15 +2709,15 @@
       <c r="L33" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M33" s="61"/>
-      <c r="N33" s="56"/>
+      <c r="M33" s="74"/>
+      <c r="N33" s="73"/>
     </row>
     <row r="34" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="62"/>
-      <c r="B34" s="63"/>
-      <c r="C34" s="64"/>
-      <c r="D34" s="65"/>
-      <c r="E34" s="66"/>
+      <c r="A34" s="61"/>
+      <c r="B34" s="75"/>
+      <c r="C34" s="76"/>
+      <c r="D34" s="77"/>
+      <c r="E34" s="78"/>
       <c r="F34" s="4" t="s">
         <v>66</v>
       </c>
@@ -2628,15 +2733,15 @@
       <c r="L34" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M34" s="61"/>
-      <c r="N34" s="56"/>
+      <c r="M34" s="74"/>
+      <c r="N34" s="73"/>
     </row>
     <row r="35" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="62"/>
-      <c r="B35" s="63"/>
-      <c r="C35" s="64"/>
-      <c r="D35" s="65"/>
-      <c r="E35" s="66"/>
+      <c r="A35" s="61"/>
+      <c r="B35" s="75"/>
+      <c r="C35" s="76"/>
+      <c r="D35" s="77"/>
+      <c r="E35" s="78"/>
       <c r="F35" s="4" t="s">
         <v>67</v>
       </c>
@@ -2652,15 +2757,15 @@
       <c r="L35" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M35" s="61"/>
-      <c r="N35" s="56"/>
+      <c r="M35" s="74"/>
+      <c r="N35" s="73"/>
     </row>
     <row r="36" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="62"/>
-      <c r="B36" s="63"/>
-      <c r="C36" s="64"/>
-      <c r="D36" s="65"/>
-      <c r="E36" s="66"/>
+      <c r="A36" s="61"/>
+      <c r="B36" s="75"/>
+      <c r="C36" s="76"/>
+      <c r="D36" s="77"/>
+      <c r="E36" s="78"/>
       <c r="F36" s="4" t="s">
         <v>68</v>
       </c>
@@ -2676,27 +2781,27 @@
       <c r="L36" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M36" s="61"/>
-      <c r="N36" s="56"/>
+      <c r="M36" s="74"/>
+      <c r="N36" s="73"/>
     </row>
     <row r="37" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="62"/>
-      <c r="B37" s="63"/>
-      <c r="C37" s="64"/>
-      <c r="D37" s="65"/>
-      <c r="E37" s="66"/>
+      <c r="A37" s="61"/>
+      <c r="B37" s="75"/>
+      <c r="C37" s="76"/>
+      <c r="D37" s="77"/>
+      <c r="E37" s="78"/>
       <c r="F37" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="M37" s="61"/>
-      <c r="N37" s="56"/>
+      <c r="M37" s="74"/>
+      <c r="N37" s="73"/>
     </row>
     <row r="38" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="62"/>
-      <c r="B38" s="63"/>
-      <c r="C38" s="64"/>
-      <c r="D38" s="65"/>
-      <c r="E38" s="66"/>
+      <c r="A38" s="61"/>
+      <c r="B38" s="75"/>
+      <c r="C38" s="76"/>
+      <c r="D38" s="77"/>
+      <c r="E38" s="78"/>
       <c r="F38" s="4" t="s">
         <v>69</v>
       </c>
@@ -2712,15 +2817,15 @@
       <c r="L38" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="M38" s="61"/>
-      <c r="N38" s="56"/>
+      <c r="M38" s="74"/>
+      <c r="N38" s="73"/>
     </row>
     <row r="39" spans="1:14" ht="57" x14ac:dyDescent="0.2">
-      <c r="A39" s="62"/>
-      <c r="B39" s="63"/>
-      <c r="C39" s="64"/>
-      <c r="D39" s="65"/>
-      <c r="E39" s="66"/>
+      <c r="A39" s="61"/>
+      <c r="B39" s="75"/>
+      <c r="C39" s="76"/>
+      <c r="D39" s="77"/>
+      <c r="E39" s="78"/>
       <c r="F39" s="9" t="s">
         <v>70</v>
       </c>
@@ -2739,23 +2844,23 @@
       <c r="L39" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="M39" s="61"/>
-      <c r="N39" s="56"/>
+      <c r="M39" s="74"/>
+      <c r="N39" s="73"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A40" s="38" t="s">
+      <c r="A40" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="B40" s="41" t="s">
+      <c r="B40" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="C40" s="44" t="s">
+      <c r="C40" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="D40" s="47" t="s">
+      <c r="D40" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="E40" s="58" t="s">
+      <c r="E40" s="42" t="s">
         <v>23</v>
       </c>
       <c r="F40" s="4" t="s">
@@ -2776,19 +2881,19 @@
       <c r="K40" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="M40" s="35">
+      <c r="M40" s="39">
         <v>20</v>
       </c>
-      <c r="N40" s="53">
+      <c r="N40" s="36">
         <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A41" s="39"/>
-      <c r="B41" s="42"/>
-      <c r="C41" s="45"/>
-      <c r="D41" s="48"/>
-      <c r="E41" s="59"/>
+      <c r="A41" s="55"/>
+      <c r="B41" s="52"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="46"/>
+      <c r="E41" s="43"/>
       <c r="F41" s="4" t="s">
         <v>73</v>
       </c>
@@ -2807,15 +2912,15 @@
       <c r="K41" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="M41" s="36"/>
-      <c r="N41" s="54"/>
+      <c r="M41" s="40"/>
+      <c r="N41" s="37"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A42" s="39"/>
-      <c r="B42" s="42"/>
-      <c r="C42" s="45"/>
-      <c r="D42" s="48"/>
-      <c r="E42" s="59"/>
+      <c r="A42" s="55"/>
+      <c r="B42" s="52"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="43"/>
       <c r="F42" s="4" t="s">
         <v>49</v>
       </c>
@@ -2834,15 +2939,15 @@
       <c r="K42" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="M42" s="36"/>
-      <c r="N42" s="54"/>
+      <c r="M42" s="40"/>
+      <c r="N42" s="37"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A43" s="39"/>
-      <c r="B43" s="42"/>
-      <c r="C43" s="45"/>
-      <c r="D43" s="48"/>
-      <c r="E43" s="59"/>
+      <c r="A43" s="55"/>
+      <c r="B43" s="52"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="46"/>
+      <c r="E43" s="43"/>
       <c r="F43" s="4" t="s">
         <v>74</v>
       </c>
@@ -2861,15 +2966,15 @@
       <c r="K43" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="M43" s="36"/>
-      <c r="N43" s="54"/>
+      <c r="M43" s="40"/>
+      <c r="N43" s="37"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A44" s="40"/>
-      <c r="B44" s="43"/>
-      <c r="C44" s="46"/>
-      <c r="D44" s="49"/>
-      <c r="E44" s="60"/>
+      <c r="A44" s="56"/>
+      <c r="B44" s="53"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="47"/>
+      <c r="E44" s="44"/>
       <c r="F44" s="4" t="s">
         <v>75</v>
       </c>
@@ -2888,24 +2993,24 @@
       <c r="K44" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="M44" s="37"/>
-      <c r="N44" s="55"/>
+      <c r="M44" s="41"/>
+      <c r="N44" s="38"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A45" s="38" t="s">
+      <c r="A45" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="B45" s="41" t="s">
+      <c r="B45" s="51" t="s">
+        <v>180</v>
+      </c>
+      <c r="C45" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="D45" s="45" t="s">
+        <v>181</v>
+      </c>
+      <c r="E45" s="79" t="s">
         <v>182</v>
-      </c>
-      <c r="C45" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="D45" s="47" t="s">
-        <v>183</v>
-      </c>
-      <c r="E45" s="50" t="s">
-        <v>184</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>89</v>
@@ -2926,16 +3031,16 @@
       <c r="L45" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="M45" s="35">
+      <c r="M45" s="39">
         <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A46" s="39"/>
-      <c r="B46" s="42"/>
-      <c r="C46" s="45"/>
-      <c r="D46" s="48"/>
-      <c r="E46" s="51"/>
+      <c r="A46" s="55"/>
+      <c r="B46" s="52"/>
+      <c r="C46" s="49"/>
+      <c r="D46" s="46"/>
+      <c r="E46" s="80"/>
       <c r="F46" s="10" t="s">
         <v>88</v>
       </c>
@@ -2952,14 +3057,14 @@
       <c r="L46" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="M46" s="36"/>
+      <c r="M46" s="40"/>
     </row>
     <row r="47" spans="1:14" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="40"/>
-      <c r="B47" s="43"/>
-      <c r="C47" s="46"/>
-      <c r="D47" s="49"/>
-      <c r="E47" s="52"/>
+      <c r="A47" s="56"/>
+      <c r="B47" s="53"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="47"/>
+      <c r="E47" s="81"/>
       <c r="F47" s="4" t="s">
         <v>90</v>
       </c>
@@ -2979,26 +3084,472 @@
       <c r="L47" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="M47" s="37"/>
+      <c r="M47" s="41"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48" s="54" t="s">
+        <v>198</v>
+      </c>
+      <c r="B48" s="51" t="s">
+        <v>201</v>
+      </c>
+      <c r="C48" s="48" t="s">
+        <v>200</v>
+      </c>
+      <c r="D48" s="45" t="s">
+        <v>212</v>
+      </c>
+      <c r="E48" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="G48" s="5">
+        <v>1</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="I48" s="4">
+        <v>1</v>
+      </c>
+      <c r="M48" s="39">
+        <v>60</v>
+      </c>
+      <c r="N48" s="36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="156.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="55"/>
+      <c r="B49" s="52"/>
+      <c r="C49" s="49"/>
+      <c r="D49" s="46"/>
+      <c r="E49" s="43"/>
+      <c r="F49" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="G49" s="5">
+        <v>2</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="L49" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="M49" s="40"/>
+      <c r="N49" s="37"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A50" s="55"/>
+      <c r="B50" s="52"/>
+      <c r="C50" s="49"/>
+      <c r="D50" s="46"/>
+      <c r="E50" s="43"/>
+      <c r="F50" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="G50" s="5">
+        <v>4</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="J50" s="4">
+        <v>1</v>
+      </c>
+      <c r="M50" s="40"/>
+      <c r="N50" s="37"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A51" s="55"/>
+      <c r="B51" s="52"/>
+      <c r="C51" s="49"/>
+      <c r="D51" s="46"/>
+      <c r="E51" s="43"/>
+      <c r="F51" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="G51" s="5">
+        <v>5</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="J51" s="4">
+        <v>1</v>
+      </c>
+      <c r="M51" s="40"/>
+      <c r="N51" s="37"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A52" s="55"/>
+      <c r="B52" s="52"/>
+      <c r="C52" s="49"/>
+      <c r="D52" s="46"/>
+      <c r="E52" s="43"/>
+      <c r="F52" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="G52" s="5">
+        <v>6</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="I52" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J52" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K52" s="6">
+        <v>0</v>
+      </c>
+      <c r="M52" s="40"/>
+      <c r="N52" s="37"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A53" s="55"/>
+      <c r="B53" s="52"/>
+      <c r="C53" s="49"/>
+      <c r="D53" s="46"/>
+      <c r="E53" s="43"/>
+      <c r="F53" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="G53" s="5">
+        <v>7</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="J53" s="4">
+        <v>1</v>
+      </c>
+      <c r="K53" s="6">
+        <v>0</v>
+      </c>
+      <c r="M53" s="40"/>
+      <c r="N53" s="38"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A54" s="55"/>
+      <c r="B54" s="52"/>
+      <c r="C54" s="49"/>
+      <c r="D54" s="46"/>
+      <c r="E54" s="43"/>
+      <c r="M54" s="40"/>
+      <c r="N54" s="35"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A55" s="55"/>
+      <c r="B55" s="52"/>
+      <c r="C55" s="49"/>
+      <c r="D55" s="46"/>
+      <c r="E55" s="43"/>
+      <c r="F55" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="G55" s="5">
+        <v>1</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="I55" s="4">
+        <v>2</v>
+      </c>
+      <c r="M55" s="40"/>
+      <c r="N55" s="36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A56" s="55"/>
+      <c r="B56" s="52"/>
+      <c r="C56" s="49"/>
+      <c r="D56" s="46"/>
+      <c r="E56" s="43"/>
+      <c r="F56" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="G56" s="5">
+        <v>2</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="I56" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J56" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K56" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M56" s="40"/>
+      <c r="N56" s="37"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A57" s="55"/>
+      <c r="B57" s="52"/>
+      <c r="C57" s="49"/>
+      <c r="D57" s="46"/>
+      <c r="E57" s="43"/>
+      <c r="F57" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="G57" s="5">
+        <v>4</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L57" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="M57" s="40"/>
+      <c r="N57" s="37"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A58" s="55"/>
+      <c r="B58" s="52"/>
+      <c r="C58" s="49"/>
+      <c r="D58" s="46"/>
+      <c r="E58" s="43"/>
+      <c r="F58" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="G58" s="5">
+        <v>5</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="I58" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="L58" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="M58" s="40"/>
+      <c r="N58" s="37"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A59" s="55"/>
+      <c r="B59" s="52"/>
+      <c r="C59" s="49"/>
+      <c r="D59" s="46"/>
+      <c r="E59" s="43"/>
+      <c r="F59" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G59" s="5">
+        <v>6</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I59" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J59" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K59" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="M59" s="40"/>
+      <c r="N59" s="37"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A60" s="55"/>
+      <c r="B60" s="52"/>
+      <c r="C60" s="49"/>
+      <c r="D60" s="46"/>
+      <c r="E60" s="43"/>
+      <c r="F60" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G60" s="5">
+        <v>7</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I60" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J60" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K60" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="M60" s="40"/>
+      <c r="N60" s="37"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A61" s="55"/>
+      <c r="B61" s="52"/>
+      <c r="C61" s="49"/>
+      <c r="D61" s="46"/>
+      <c r="E61" s="43"/>
+      <c r="F61" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="M61" s="40"/>
+      <c r="N61" s="38"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A62" s="55"/>
+      <c r="B62" s="52"/>
+      <c r="C62" s="49"/>
+      <c r="D62" s="46"/>
+      <c r="E62" s="43"/>
+      <c r="M62" s="40"/>
+      <c r="N62" s="35"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A63" s="55"/>
+      <c r="B63" s="52"/>
+      <c r="C63" s="49"/>
+      <c r="D63" s="46"/>
+      <c r="E63" s="43"/>
+      <c r="F63" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="G63" s="5">
+        <v>1</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="I63" s="4">
+        <v>3</v>
+      </c>
+      <c r="M63" s="40"/>
+      <c r="N63" s="36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A64" s="55"/>
+      <c r="B64" s="52"/>
+      <c r="C64" s="49"/>
+      <c r="D64" s="46"/>
+      <c r="E64" s="43"/>
+      <c r="F64" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G64" s="5">
+        <v>2</v>
+      </c>
+      <c r="H64" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I64" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="J64" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K64" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="M64" s="40"/>
+      <c r="N64" s="37"/>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A65" s="55"/>
+      <c r="B65" s="52"/>
+      <c r="C65" s="49"/>
+      <c r="D65" s="46"/>
+      <c r="E65" s="43"/>
+      <c r="F65" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G65" s="5">
+        <v>4</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I65" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="J65" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="K65" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="M65" s="40"/>
+      <c r="N65" s="37"/>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A66" s="55"/>
+      <c r="B66" s="52"/>
+      <c r="C66" s="49"/>
+      <c r="D66" s="46"/>
+      <c r="E66" s="43"/>
+      <c r="F66" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G66" s="5">
+        <v>6</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I66" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="J66" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="K66" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="M66" s="40"/>
+      <c r="N66" s="37"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A67" s="56"/>
+      <c r="B67" s="53"/>
+      <c r="C67" s="50"/>
+      <c r="D67" s="47"/>
+      <c r="E67" s="44"/>
+      <c r="F67" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="M67" s="41"/>
+      <c r="N67" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="M3:M16"/>
-    <mergeCell ref="N3:N16"/>
-    <mergeCell ref="F5:F12"/>
-    <mergeCell ref="F1:L1"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="A3:A16"/>
-    <mergeCell ref="B3:B16"/>
-    <mergeCell ref="C3:C16"/>
-    <mergeCell ref="D3:D16"/>
-    <mergeCell ref="E3:E16"/>
+  <mergeCells count="46">
+    <mergeCell ref="M45:M47"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="D45:D47"/>
+    <mergeCell ref="E45:E47"/>
     <mergeCell ref="N40:N44"/>
     <mergeCell ref="N17:N39"/>
     <mergeCell ref="F19:F26"/>
@@ -3014,12 +3565,31 @@
     <mergeCell ref="C17:C39"/>
     <mergeCell ref="D17:D39"/>
     <mergeCell ref="E17:E39"/>
-    <mergeCell ref="M45:M47"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="D45:D47"/>
-    <mergeCell ref="E45:E47"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="M3:M16"/>
+    <mergeCell ref="N3:N16"/>
+    <mergeCell ref="F5:F12"/>
+    <mergeCell ref="F1:L1"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="E3:E16"/>
+    <mergeCell ref="D48:D67"/>
+    <mergeCell ref="C48:C67"/>
+    <mergeCell ref="B48:B67"/>
+    <mergeCell ref="A48:A67"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="A3:A16"/>
+    <mergeCell ref="B3:B16"/>
+    <mergeCell ref="C3:C16"/>
+    <mergeCell ref="D3:D16"/>
+    <mergeCell ref="N48:N53"/>
+    <mergeCell ref="M48:M67"/>
+    <mergeCell ref="N55:N61"/>
+    <mergeCell ref="N63:N67"/>
+    <mergeCell ref="E48:E67"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A1:XFD1">
@@ -3059,20 +3629,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="82" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="85" t="s">
         <v>126</v>
       </c>
-      <c r="C1" s="85"/>
-      <c r="D1" s="82" t="s">
+      <c r="C1" s="86"/>
+      <c r="D1" s="83" t="s">
         <v>121</v>
       </c>
-      <c r="E1" s="82"/>
+      <c r="E1" s="83"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="81"/>
+      <c r="A2" s="82"/>
       <c r="B2" s="29" t="s">
         <v>127</v>
       </c>
@@ -3087,7 +3657,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="84" t="s">
         <v>105</v>
       </c>
       <c r="B3" s="22" t="s">
@@ -3104,7 +3674,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="83"/>
+      <c r="A4" s="84"/>
       <c r="B4" s="22" t="s">
         <v>109</v>
       </c>
@@ -3119,7 +3689,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="83"/>
+      <c r="A5" s="84"/>
       <c r="B5" s="22" t="s">
         <v>112</v>
       </c>
@@ -3134,7 +3704,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="83"/>
+      <c r="A6" s="84"/>
       <c r="B6" s="22" t="s">
         <v>115</v>
       </c>
@@ -3149,7 +3719,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="83"/>
+      <c r="A7" s="84"/>
       <c r="B7" s="22" t="s">
         <v>118</v>
       </c>
@@ -3185,7 +3755,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3207,13 +3777,13 @@
         <v>129</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D1" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" s="31" t="s">
         <v>164</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>166</v>
       </c>
       <c r="F1" s="31" t="s">
         <v>130</v>
@@ -3222,30 +3792,30 @@
         <v>134</v>
       </c>
       <c r="H1" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="J1" s="31" t="s">
         <v>179</v>
       </c>
-      <c r="I1" s="31" t="s">
-        <v>180</v>
-      </c>
-      <c r="J1" s="31" t="s">
-        <v>181</v>
-      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="87" t="s">
         <v>131</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>132</v>
       </c>
       <c r="C2" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="E2" s="31" t="s">
         <v>165</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>153</v>
-      </c>
-      <c r="E2" s="31" t="s">
-        <v>167</v>
       </c>
       <c r="F2" s="31" t="s">
         <v>133</v>
@@ -3257,28 +3827,28 @@
         <v>136</v>
       </c>
       <c r="I2" s="32" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J2" s="32" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="86"/>
+      <c r="A3" s="87"/>
       <c r="B3" s="31" t="s">
         <v>137</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F3" s="31" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G3" s="31" t="s">
         <v>135</v>
@@ -3287,25 +3857,25 @@
         <v>138</v>
       </c>
       <c r="I3" s="32" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J3" s="32" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="86"/>
+      <c r="A4" s="87"/>
       <c r="B4" s="31" t="s">
         <v>139</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F4" s="31" t="s">
         <v>140</v>
@@ -3317,180 +3887,180 @@
         <v>138</v>
       </c>
       <c r="I4" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="J4" s="32" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="87" t="s">
+        <v>221</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="I5" s="32" t="s">
         <v>158</v>
       </c>
-      <c r="J4" s="32" t="s">
+      <c r="J5" s="32" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="87"/>
+      <c r="B6" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>219</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="H6" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="I6" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="J6" s="32" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="87"/>
+      <c r="B7" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>220</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="H7" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="I7" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="J7" s="32" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="87"/>
+      <c r="B8" s="31" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="86" t="s">
-        <v>141</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>142</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="D5" s="31" t="s">
+      <c r="C8" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="E5" s="31" t="s">
-        <v>171</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>143</v>
-      </c>
-      <c r="G5" s="31" t="s">
-        <v>144</v>
-      </c>
-      <c r="H5" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="I5" s="32" t="s">
-        <v>160</v>
-      </c>
-      <c r="J5" s="32" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="86"/>
-      <c r="B6" s="31" t="s">
-        <v>146</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>149</v>
-      </c>
-      <c r="D6" s="31" t="s">
-        <v>173</v>
-      </c>
-      <c r="E6" s="31" t="s">
+      <c r="E8" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="F6" s="31" t="s">
-        <v>147</v>
-      </c>
-      <c r="G6" s="31" t="s">
-        <v>148</v>
-      </c>
-      <c r="H6" s="32" t="s">
-        <v>150</v>
-      </c>
-      <c r="I6" s="32" t="s">
-        <v>160</v>
-      </c>
-      <c r="J6" s="32" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="86"/>
-      <c r="B7" s="31" t="s">
-        <v>151</v>
-      </c>
-      <c r="C7" s="31" t="s">
+      <c r="F8" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="I8" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="J8" s="32" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="87"/>
+      <c r="B9" s="31" t="s">
+        <v>191</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>190</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>192</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>193</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>194</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="H9" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="I9" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="J9" s="32" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="87"/>
+      <c r="B10" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="E10" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="D7" s="31" t="s">
-        <v>174</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>176</v>
-      </c>
-      <c r="F7" s="31" t="s">
-        <v>152</v>
-      </c>
-      <c r="G7" s="31" t="s">
-        <v>148</v>
-      </c>
-      <c r="H7" s="32" t="s">
-        <v>150</v>
-      </c>
-      <c r="I7" s="32" t="s">
-        <v>160</v>
-      </c>
-      <c r="J7" s="32" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="86"/>
-      <c r="B8" s="31" t="s">
-        <v>161</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>172</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>177</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="G8" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="H8" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="I8" s="32" t="s">
-        <v>160</v>
-      </c>
-      <c r="J8" s="32" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="86"/>
-      <c r="B9" s="31" t="s">
-        <v>195</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>194</v>
-      </c>
-      <c r="D9" s="31" t="s">
-        <v>196</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="F9" s="31" t="s">
-        <v>198</v>
-      </c>
-      <c r="G9" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="H9" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="I9" s="32" t="s">
-        <v>199</v>
-      </c>
-      <c r="J9" s="32" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="86"/>
-      <c r="B10" s="33" t="s">
-        <v>186</v>
-      </c>
-      <c r="C10" s="33" t="s">
+      <c r="F10" s="31" t="s">
         <v>187</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>172</v>
-      </c>
-      <c r="E10" s="33" t="s">
-        <v>189</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>191</v>
       </c>
       <c r="G10" s="31" t="s">
         <v>135</v>
@@ -3506,21 +4076,21 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="86"/>
+      <c r="A11" s="87"/>
       <c r="B11" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="E11" s="33" t="s">
         <v>186</v>
       </c>
-      <c r="C11" s="33" t="s">
-        <v>187</v>
-      </c>
-      <c r="D11" s="31" t="s">
-        <v>172</v>
-      </c>
-      <c r="E11" s="33" t="s">
-        <v>190</v>
-      </c>
       <c r="F11" s="31" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="G11" s="31" t="s">
         <v>135</v>
@@ -3536,18 +4106,18 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="86"/>
+      <c r="A12" s="87"/>
       <c r="B12" s="33" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="31" t="s">

</xml_diff>

<commit_message>
feat(CAN): add mcMessage content to CAN and model
</commit_message>
<xml_diff>
--- a/doc/Fury-CAN-protocol/fury-CAN-protocol.v2.1.xlsx
+++ b/doc/Fury-CAN-protocol/fury-CAN-protocol.v2.1.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="186">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -1620,56 +1620,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">正常</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">报警</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">解析见电控通信协议</t>
-    </r>
+    <t xml:space="preserve">控制器就绪, 预充状态, 旋变报警, 过流报警, 母线过压, 控制点异常, 母线欠压, 功率限幅报警</t>
   </si>
   <si>
     <r>
@@ -1692,6 +1643,9 @@
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">控制器温度报警, 电机温度报警</t>
   </si>
   <si>
     <t xml:space="preserve">0x186040F3</t>
@@ -2813,8 +2767,8 @@
   </sheetPr>
   <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J52" activeCellId="0" sqref="J52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F36" colorId="64" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L61" activeCellId="0" sqref="L61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4342,7 +4296,7 @@
       <c r="M56" s="30"/>
       <c r="N56" s="31"/>
     </row>
-    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="41"/>
       <c r="B57" s="45"/>
       <c r="C57" s="23"/>
@@ -4362,13 +4316,13 @@
       </c>
       <c r="J57" s="26"/>
       <c r="K57" s="28"/>
-      <c r="L57" s="26" t="s">
+      <c r="L57" s="29" t="s">
         <v>117</v>
       </c>
       <c r="M57" s="30"/>
       <c r="N57" s="31"/>
     </row>
-    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="41"/>
       <c r="B58" s="45"/>
       <c r="C58" s="23"/>
@@ -4389,7 +4343,7 @@
       <c r="J58" s="26"/>
       <c r="K58" s="28"/>
       <c r="L58" s="26" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="M58" s="30"/>
       <c r="N58" s="31"/>
@@ -4611,22 +4565,22 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="41" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B68" s="45" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C68" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D68" s="24" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E68" s="25" t="s">
         <v>75</v>
       </c>
       <c r="F68" s="26" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G68" s="7" t="n">
         <v>1</v>
@@ -4635,7 +4589,7 @@
         <v>21</v>
       </c>
       <c r="I68" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J68" s="6" t="s">
         <v>47</v>
@@ -4651,7 +4605,7 @@
       <c r="D69" s="24"/>
       <c r="E69" s="25"/>
       <c r="F69" s="26" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G69" s="7" t="n">
         <v>3</v>
@@ -4660,13 +4614,13 @@
         <v>21</v>
       </c>
       <c r="I69" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J69" s="6" t="s">
         <v>85</v>
       </c>
       <c r="K69" s="7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4676,7 +4630,7 @@
       <c r="D70" s="24"/>
       <c r="E70" s="25"/>
       <c r="F70" s="26" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G70" s="7" t="n">
         <v>5</v>
@@ -4685,7 +4639,7 @@
         <v>77</v>
       </c>
       <c r="I70" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="J70" s="49" t="n">
         <v>0.01</v>
@@ -4696,22 +4650,22 @@
     </row>
     <row r="71" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="41" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B71" s="45" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C71" s="48" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D71" s="24" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E71" s="46" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F71" s="26" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G71" s="7" t="n">
         <v>1</v>
@@ -4720,33 +4674,33 @@
         <v>77</v>
       </c>
       <c r="I71" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J71" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K71" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="51" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C72" s="48" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D72" s="24" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E72" s="46" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F72" s="26" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G72" s="7" t="n">
         <v>1</v>
@@ -4755,13 +4709,13 @@
         <v>21</v>
       </c>
       <c r="I72" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J72" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K72" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4886,48 +4840,48 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="52" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C1" s="53" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D1" s="53" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E1" s="53" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F1" s="52" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="53" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H1" s="53" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I1" s="53" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J1" s="53" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="54" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B2" s="52" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C2" s="52" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="53" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E2" s="53" t="s">
         <v>26</v>
@@ -4936,316 +4890,316 @@
         <v>15</v>
       </c>
       <c r="G2" s="53" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H2" s="55" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I2" s="55" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="J2" s="55" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="54"/>
       <c r="B3" s="52" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C3" s="53" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D3" s="52" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="53" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F3" s="52" t="s">
         <v>49</v>
       </c>
       <c r="G3" s="53" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H3" s="55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I3" s="55" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="J3" s="55" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="54"/>
       <c r="B4" s="52" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C4" s="53" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D4" s="52" t="s">
         <v>18</v>
       </c>
       <c r="E4" s="53" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F4" s="52" t="s">
         <v>73</v>
       </c>
       <c r="G4" s="53" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H4" s="55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I4" s="55" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="J4" s="55" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="54" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C5" s="52" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="53" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E5" s="53" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F5" s="52" t="s">
         <v>104</v>
       </c>
       <c r="G5" s="53" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H5" s="55" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I5" s="55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J5" s="55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="54"/>
       <c r="B6" s="52" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C6" s="52" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D6" s="53" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E6" s="53" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G6" s="53" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H6" s="55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I6" s="55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J6" s="55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="54"/>
       <c r="B7" s="52" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C7" s="52" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D7" s="53" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E7" s="53" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G7" s="53" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H7" s="55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I7" s="55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J7" s="55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="54"/>
       <c r="B8" s="52" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C8" s="53" t="s">
         <v>90</v>
       </c>
       <c r="D8" s="53" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F8" s="52" t="s">
         <v>88</v>
       </c>
       <c r="G8" s="53" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H8" s="55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I8" s="55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J8" s="55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="54"/>
       <c r="B9" s="52" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C9" s="52" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E9" s="53" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F9" s="52" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G9" s="53" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H9" s="55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I9" s="55" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="J9" s="55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="54"/>
       <c r="B10" s="53" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C10" s="52" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D10" s="53" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E10" s="53" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F10" s="52" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G10" s="53" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H10" s="55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I10" s="55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J10" s="55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="54"/>
       <c r="B11" s="53" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C11" s="52" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E11" s="53" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F11" s="52" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G11" s="53" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H11" s="55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I11" s="55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J11" s="55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="54"/>
       <c r="B12" s="53" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C12" s="52" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E12" s="56" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F12" s="56"/>
       <c r="G12" s="53" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H12" s="55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I12" s="55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J12" s="55" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(bus): fix allFlag and mcMessage reading overstep bug
</commit_message>
<xml_diff>
--- a/doc/Fury-CAN-protocol/fury-CAN-protocol.v2.1.xlsx
+++ b/doc/Fury-CAN-protocol/fury-CAN-protocol.v2.1.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="189">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -1646,6 +1646,15 @@
   </si>
   <si>
     <t xml:space="preserve">控制器温度报警, 电机温度报警</t>
+  </si>
+  <si>
+    <t xml:space="preserve">继电器状态</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0/1/2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0: 异常 1: 正常未激活 2: 正常激活</t>
   </si>
   <si>
     <t xml:space="preserve">0x186040F3</t>
@@ -2767,7 +2776,7 @@
   </sheetPr>
   <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F36" colorId="64" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L61" activeCellId="0" sqref="L61"/>
     </sheetView>
   </sheetViews>
@@ -4404,20 +4413,29 @@
       <c r="M60" s="30"/>
       <c r="N60" s="31"/>
     </row>
-    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="16.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="41"/>
       <c r="B61" s="45"/>
       <c r="C61" s="23"/>
       <c r="D61" s="24"/>
       <c r="E61" s="46"/>
       <c r="F61" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="H61" s="26"/>
-      <c r="I61" s="26"/>
+        <v>120</v>
+      </c>
+      <c r="G61" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="H61" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="I61" s="26" t="s">
+        <v>121</v>
+      </c>
       <c r="J61" s="26"/>
       <c r="K61" s="28"/>
-      <c r="L61" s="26"/>
+      <c r="L61" s="26" t="s">
+        <v>122</v>
+      </c>
       <c r="M61" s="30"/>
       <c r="N61" s="31"/>
     </row>
@@ -4565,22 +4583,22 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="41" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B68" s="45" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C68" s="48" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D68" s="24" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E68" s="25" t="s">
         <v>75</v>
       </c>
       <c r="F68" s="26" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G68" s="7" t="n">
         <v>1</v>
@@ -4589,7 +4607,7 @@
         <v>21</v>
       </c>
       <c r="I68" s="6" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="J68" s="6" t="s">
         <v>47</v>
@@ -4605,7 +4623,7 @@
       <c r="D69" s="24"/>
       <c r="E69" s="25"/>
       <c r="F69" s="26" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="G69" s="7" t="n">
         <v>3</v>
@@ -4614,13 +4632,13 @@
         <v>21</v>
       </c>
       <c r="I69" s="6" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="J69" s="6" t="s">
         <v>85</v>
       </c>
       <c r="K69" s="7" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4630,7 +4648,7 @@
       <c r="D70" s="24"/>
       <c r="E70" s="25"/>
       <c r="F70" s="26" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="G70" s="7" t="n">
         <v>5</v>
@@ -4639,7 +4657,7 @@
         <v>77</v>
       </c>
       <c r="I70" s="6" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="J70" s="49" t="n">
         <v>0.01</v>
@@ -4650,22 +4668,22 @@
     </row>
     <row r="71" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="41" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B71" s="45" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C71" s="48" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D71" s="24" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E71" s="46" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F71" s="26" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G71" s="7" t="n">
         <v>1</v>
@@ -4674,33 +4692,33 @@
         <v>77</v>
       </c>
       <c r="I71" s="6" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="J71" s="6" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="K71" s="7" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="51" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C72" s="48" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D72" s="24" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E72" s="46" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F72" s="26" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G72" s="7" t="n">
         <v>1</v>
@@ -4709,13 +4727,13 @@
         <v>21</v>
       </c>
       <c r="I72" s="6" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="J72" s="6" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="K72" s="7" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4840,48 +4858,48 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="52" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C1" s="53" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D1" s="53" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E1" s="53" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="F1" s="52" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="53" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H1" s="53" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="I1" s="53" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="J1" s="53" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="54" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B2" s="52" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C2" s="52" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="53" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="E2" s="53" t="s">
         <v>26</v>
@@ -4890,316 +4908,316 @@
         <v>15</v>
       </c>
       <c r="G2" s="53" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="H2" s="55" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="I2" s="55" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="J2" s="55" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="54"/>
       <c r="B3" s="52" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C3" s="53" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="D3" s="52" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="53" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="F3" s="52" t="s">
         <v>49</v>
       </c>
       <c r="G3" s="53" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="H3" s="55" t="s">
+        <v>165</v>
+      </c>
+      <c r="I3" s="55" t="s">
         <v>162</v>
       </c>
-      <c r="I3" s="55" t="s">
-        <v>159</v>
-      </c>
       <c r="J3" s="55" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="54"/>
       <c r="B4" s="52" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C4" s="53" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="D4" s="52" t="s">
         <v>18</v>
       </c>
       <c r="E4" s="53" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="F4" s="52" t="s">
         <v>73</v>
       </c>
       <c r="G4" s="53" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="H4" s="55" t="s">
+        <v>165</v>
+      </c>
+      <c r="I4" s="55" t="s">
         <v>162</v>
       </c>
-      <c r="I4" s="55" t="s">
-        <v>159</v>
-      </c>
       <c r="J4" s="55" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="54" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C5" s="52" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="53" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="E5" s="53" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="F5" s="52" t="s">
         <v>104</v>
       </c>
       <c r="G5" s="53" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="H5" s="55" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="I5" s="55" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="J5" s="55" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="54"/>
       <c r="B6" s="52" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C6" s="52" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D6" s="53" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E6" s="53" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="G6" s="53" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="H6" s="55" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="I6" s="55" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="J6" s="55" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="54"/>
       <c r="B7" s="52" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C7" s="52" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D7" s="53" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E7" s="53" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="G7" s="53" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="H7" s="55" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="I7" s="55" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="J7" s="55" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="54"/>
       <c r="B8" s="52" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C8" s="53" t="s">
         <v>90</v>
       </c>
       <c r="D8" s="53" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F8" s="52" t="s">
         <v>88</v>
       </c>
       <c r="G8" s="53" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="H8" s="55" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="I8" s="55" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="J8" s="55" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="54"/>
       <c r="B9" s="52" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C9" s="52" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="E9" s="53" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="F9" s="52" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="G9" s="53" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="H9" s="55" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="I9" s="55" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="J9" s="55" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="54"/>
       <c r="B10" s="53" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C10" s="52" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D10" s="53" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E10" s="53" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F10" s="52" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="G10" s="53" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="H10" s="55" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="I10" s="55" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="J10" s="55" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="54"/>
       <c r="B11" s="53" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C11" s="52" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E11" s="53" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="F11" s="52" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="G11" s="53" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="H11" s="55" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="I11" s="55" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="J11" s="55" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="54"/>
       <c r="B12" s="53" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C12" s="52" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E12" s="56" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="F12" s="56"/>
       <c r="G12" s="53" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="H12" s="55" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="I12" s="55" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="J12" s="55" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>